<commit_message>
Checking in changes to common_defs.json
</commit_message>
<xml_diff>
--- a/utils/document/common_defs.xlsx
+++ b/utils/document/common_defs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="73">
   <si>
     <t>Field Name</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>resourceId</t>
+  </si>
+  <si>
+    <t>id of the resource in the resource server</t>
   </si>
   <si>
     <t>name</t>
@@ -575,7 +581,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -672,7 +678,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="20" customHeight="1">
@@ -681,7 +687,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20" customHeight="1">
@@ -695,7 +701,7 @@
     </row>
     <row r="14" spans="1:3" ht="20" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="20" customHeight="1">
@@ -704,7 +710,7 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="20" customHeight="1">
@@ -736,7 +742,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="20" customHeight="1">
@@ -768,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="20" customHeight="1">
@@ -800,7 +806,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="20" customHeight="1">
@@ -818,12 +824,12 @@
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="20" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="20" customHeight="1">
@@ -841,7 +847,7 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="20" customHeight="1">
@@ -850,7 +856,7 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="20" customHeight="1">
@@ -896,7 +902,7 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="20" customHeight="1">
@@ -905,7 +911,7 @@
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="20" customHeight="1">
@@ -914,12 +920,12 @@
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="20" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="20" customHeight="1">
@@ -928,7 +934,7 @@
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="20" customHeight="1">
@@ -937,7 +943,7 @@
         <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="20" customHeight="1">
@@ -946,7 +952,7 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="20" customHeight="1">
@@ -960,7 +966,7 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="20" customHeight="1">
@@ -978,7 +984,7 @@
         <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="20" customHeight="1">
@@ -992,7 +998,7 @@
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="20" customHeight="1">
@@ -1010,7 +1016,7 @@
         <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="20" customHeight="1">
@@ -1056,7 +1062,7 @@
         <v>4</v>
       </c>
       <c r="C59" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="20" customHeight="1">
@@ -1074,7 +1080,7 @@
         <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="20" customHeight="1">
@@ -1088,7 +1094,7 @@
         <v>4</v>
       </c>
       <c r="C63" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="20" customHeight="1">
@@ -1106,7 +1112,7 @@
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="20" customHeight="1">
@@ -1119,6 +1125,9 @@
       <c r="B67" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C67" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="68" spans="1:3" ht="20" customHeight="1">
       <c r="A68" s="1"/>
@@ -1135,7 +1144,7 @@
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="20" customHeight="1">
@@ -1149,7 +1158,7 @@
         <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="20" customHeight="1">
@@ -1158,7 +1167,7 @@
         <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="20" customHeight="1">
@@ -1167,12 +1176,12 @@
         <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="20" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="20" customHeight="1">
@@ -1181,7 +1190,7 @@
         <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="20" customHeight="1">
@@ -1190,7 +1199,7 @@
         <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="20" customHeight="1">
@@ -1199,7 +1208,7 @@
         <v>8</v>
       </c>
       <c r="C77" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="20" customHeight="1">
@@ -1213,7 +1222,7 @@
         <v>4</v>
       </c>
       <c r="C79" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="20" customHeight="1">
@@ -1231,7 +1240,7 @@
         <v>8</v>
       </c>
       <c r="C81" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="20" customHeight="1">
@@ -1263,7 +1272,7 @@
         <v>8</v>
       </c>
       <c r="C85" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="20" customHeight="1">
@@ -1295,7 +1304,7 @@
         <v>8</v>
       </c>
       <c r="C89" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="20" customHeight="1">
@@ -1327,7 +1336,7 @@
         <v>8</v>
       </c>
       <c r="C93" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="20" customHeight="1">
@@ -1340,6 +1349,9 @@
       <c r="B95" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C95" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="96" spans="1:3" ht="20" customHeight="1">
       <c r="A96" s="1"/>
@@ -1370,7 +1382,7 @@
         <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="20" customHeight="1">
@@ -1388,7 +1400,7 @@
         <v>8</v>
       </c>
       <c r="C101" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="20" customHeight="1">
@@ -1402,7 +1414,7 @@
         <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="20" customHeight="1">
@@ -1420,7 +1432,7 @@
         <v>8</v>
       </c>
       <c r="C105" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="20" customHeight="1">
@@ -1433,6 +1445,9 @@
       <c r="B107" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="108" spans="1:3" ht="20" customHeight="1">
       <c r="A108" s="1"/>
@@ -1449,7 +1464,7 @@
         <v>8</v>
       </c>
       <c r="C109" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="20" customHeight="1">
@@ -1481,7 +1496,7 @@
         <v>8</v>
       </c>
       <c r="C113" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="20" customHeight="1">
@@ -1494,21 +1509,53 @@
       <c r="B115" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C115" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="116" spans="1:3" ht="20" customHeight="1">
       <c r="A116" s="1"/>
       <c r="B116" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C116" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="117" spans="1:3" ht="20" customHeight="1">
       <c r="A117" s="1"/>
       <c r="B117" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C117" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="20" customHeight="1">
+      <c r="A118" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="20" customHeight="1">
+      <c r="A119" s="1"/>
+      <c r="B119" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="20" customHeight="1">
+      <c r="A120" s="1"/>
+      <c r="B120" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="20" customHeight="1">
+      <c r="A121" s="1"/>
+      <c r="B121" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="30">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A13"/>
@@ -1538,6 +1585,7 @@
     <mergeCell ref="A106:A109"/>
     <mergeCell ref="A110:A113"/>
     <mergeCell ref="A114:A117"/>
+    <mergeCell ref="A118:A121"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added traffic data models
</commit_message>
<xml_diff>
--- a/utils/document/common_defs.xlsx
+++ b/utils/document/common_defs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="73">
   <si>
     <t>Field Name</t>
   </si>
@@ -115,7 +115,7 @@
     <t>Link to the base schema for this itemType</t>
   </si>
   <si>
-    <t>iri</t>
+    <t>IRI</t>
   </si>
   <si>
     <t>resourceServer</t>
@@ -663,6 +663,9 @@
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="20" customHeight="1">
       <c r="A10" s="1" t="s">

</xml_diff>